<commit_message>
removed ICPetcdHighNumberOfFailedGRPCRequests because of false alerts on ICP
</commit_message>
<xml_diff>
--- a/prometheus/alerts_icp_2.1.0.2-3.1.1/ICP_Prometheus_alerts.xlsx
+++ b/prometheus/alerts_icp_2.1.0.2-3.1.1/ICP_Prometheus_alerts.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10309"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10715"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rafalszypulka/GitHub/CSMO-ICP/prometheus/alerts_icp_3.1.2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rafalszypulka/GitHub/CSMO-ICP/prometheus/alerts_icp_2.1.0.2-3.1.1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA41A2B7-21D4-F749-8916-7DE72F22D398}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32199C93-B768-3545-94AC-3E9CBD983768}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1040" yWindow="1680" windowWidth="27760" windowHeight="15200" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="119">
   <si>
     <t>Alert Name</t>
   </si>
@@ -1250,15 +1250,6 @@
     <t>etcd instance {{ $labels.instance }} has seen {{ $value }} leader changes within the last hour</t>
   </si>
   <si>
-    <t>ICPetcdHighNumberOfFailedGRPCRequests</t>
-  </si>
-  <si>
-    <t>a high number of gRPC requests are failing</t>
-  </si>
-  <si>
-    <t>{{ $value }}% of requests for {{ $labels.grpc_method }} failed on etcd instance {{ $labels.instance }}</t>
-  </si>
-  <si>
     <t>ICPetcdHighNumberOfFailedProposals</t>
   </si>
   <si>
@@ -1293,12 +1284,6 @@
   </si>
   <si>
     <t>Applicable only for etcd clusters. The alert is fired if there are lots of leader changes</t>
-  </si>
-  <si>
-    <t>Alert if more than 1% of gRPC method calls for etcd have failed within the last 5 minutes. Check etcd logs.</t>
-  </si>
-  <si>
-    <t>Alert if more than 5% of gRPC method calls for etcd have failed within the last 5 minutes. Check etcd logs</t>
   </si>
   <si>
     <t>Writes and configuration changes sent to etcd are called proposals. The raft protocol ensures that the proposals are applied correctly to the cluster. Rate of failed proposals should be low. Check etcd logs.</t>
@@ -1712,10 +1697,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E33"/>
+  <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A29" sqref="A29:XFD30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1780,7 +1765,7 @@
     </row>
     <row r="4" spans="1:5" ht="85" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>13</v>
@@ -2069,7 +2054,7 @@
     </row>
     <row r="21" spans="1:5" ht="36" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>6</v>
@@ -2086,7 +2071,7 @@
     </row>
     <row r="22" spans="1:5" ht="51" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>6</v>
@@ -2137,7 +2122,7 @@
     </row>
     <row r="25" spans="1:5" ht="71" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>6</v>
@@ -2166,7 +2151,7 @@
         <v>94</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="17" x14ac:dyDescent="0.2">
@@ -2183,7 +2168,7 @@
         <v>97</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="51" x14ac:dyDescent="0.2">
@@ -2200,7 +2185,7 @@
         <v>100</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="51" x14ac:dyDescent="0.2">
@@ -2217,75 +2202,41 @@
         <v>103</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="51" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="51" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>6</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" ht="51" x14ac:dyDescent="0.2">
-      <c r="A32" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="B32" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C32" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="D32" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="E32" s="5" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" ht="51" x14ac:dyDescent="0.2">
-      <c r="A33" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="B33" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C33" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="D33" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="E33" s="5" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
     </row>
   </sheetData>

</xml_diff>